<commit_message>
fixed officer photo ratio
</commit_message>
<xml_diff>
--- a/public/officer_page/page_officer_data.xlsx
+++ b/public/officer_page/page_officer_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15413\Desktop\psu_shpe_website-main\psu_shpe_website-main\public\officer_page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72161726-0A19-448C-9D44-0B789E6304BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9193E8B2-5312-4F94-A426-EE07583B25AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="4830" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="61695" yWindow="8325" windowWidth="28800" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -500,7 +500,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -763,28 +763,28 @@
     <mergeCell ref="D19:E19"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D11" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D12" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E12" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D13" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="E13" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D9" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D10" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D11" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D12" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E12" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D13" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E13" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D2" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>